<commit_message>
render links in pandas html table
Signed-off-by: Caleb Grant <geocoug@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/static/workouts.xlsx
+++ b/docs/static/workouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgrant/Library/Mobile Documents/com~apple~CloudDocs/GitHub/geocoug/toolkit/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgrant/GitHub/geocoug/toolkit/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F60AD-BCE1-8340-A83A-A5F3C34696A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FCE1AD-679E-2F46-B1CC-57B519BFC52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24280" xr2:uid="{33B94D11-EE83-ED43-B23D-BCAC305DFE17}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24280" activeTab="7" xr2:uid="{33B94D11-EE83-ED43-B23D-BCAC305DFE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Back-Biceps" sheetId="1" r:id="rId1"/>
@@ -242,66 +242,6 @@
     <t>Bird Dog</t>
   </si>
   <si>
-    <t>&lt;a href="https://weighttraining.guide/exercises/barbell-deadlift/"&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/dumbbell-squat/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/standing-dumbbell-one-leg-calf-raise/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/hyperextension/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.verywellfit.com/how-to-do-the-bird-dog-exercise-3498253'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/straight-back-seated-cable-row/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/bent-over-dumbbell-row/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/dumbbell-wide-grip-upright-row/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/seated-alternating-dumbbell-curl/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/dumbbell-hammer-curl/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/dumbbell-farmers-walk/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/dumbbell-bench-press/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/incline-dumbbell-bench-press/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/dumbbell-fly/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/cable-one-arm-lateral-raise/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/seated-dumbbell-front-raise/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/triceps-push-down/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/front-plank/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/sit-up/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://weighttraining.guide/exercises/seated-knee-raise/'&gt;View&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Leg Kickbacks</t>
   </si>
   <si>
@@ -336,6 +276,66 @@
   </si>
   <si>
     <t>Face Pulls</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/seated-knee-raise/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/dumbbell-bench-press/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/incline-dumbbell-bench-press/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/dumbbell-fly/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/cable-one-arm-lateral-raise/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/seated-dumbbell-front-raise/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/triceps-push-down/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/front-plank/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/sit-up/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/straight-back-seated-cable-row/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/bent-over-dumbbell-row/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/dumbbell-wide-grip-upright-row/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/seated-alternating-dumbbell-curl/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/dumbbell-hammer-curl/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/dumbbell-farmers-walk/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/barbell-deadlift/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/dumbbell-squat/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/standing-dumbbell-one-leg-calf-raise/)</t>
+  </si>
+  <si>
+    <t>[View](https://weighttraining.guide/exercises/hyperextension/)</t>
+  </si>
+  <si>
+    <t>[View](https://www.verywellfit.com/how-to-do-the-bird-dog-exercise-3498253)</t>
   </si>
 </sst>
 </file>
@@ -394,11 +394,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +418,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -705,7 +706,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -715,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF3C11C-73CE-304C-B13C-F9FD3DC9A2A4}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +779,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -969,7 +970,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -980,7 +981,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1061,7 +1062,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1228,18 +1229,18 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1250,7 +1251,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1313,19 +1314,19 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
         <v>46</v>
@@ -1339,19 +1340,19 @@
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
@@ -1365,19 +1366,19 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
         <v>46</v>
@@ -1391,19 +1392,19 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
         <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
         <v>46</v>
@@ -1419,7 +1420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66115A2-F7BB-0142-8BE6-1212D3F4745D}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
@@ -1448,7 +1451,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -1462,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -1476,7 +1479,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -1490,7 +1493,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
@@ -1504,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -1518,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17">
@@ -1532,7 +1535,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
@@ -1546,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
@@ -1559,8 +1562,8 @@
       <c r="C10" s="2">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>85</v>
+      <c r="D10" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1573,10 +1576,13 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17">
       <c r="A1" s="1" t="s">
@@ -1603,7 +1609,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -1617,7 +1623,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -1631,7 +1637,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -1645,7 +1651,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
@@ -1659,7 +1665,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -1673,7 +1679,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1685,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA328CD7-D52E-6148-98AF-351AC996FD22}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1716,7 +1722,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -1730,7 +1736,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -1744,7 +1750,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -1770,7 +1776,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -1784,7 +1790,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>